<commit_message>
feat(backend): add login functionality
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,23 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>hello21</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(UI): jump back to login page after registration
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,74 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>arya</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>aryan</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>aryan21</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>aryan</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sisodiya14</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Abhishek Sisodiya</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>abhay</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>abhay</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(backend): saving plot image in local
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,6 +616,40 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>xyz123</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Abhishek Sisodiyha</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2232</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>vijay123</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Vijay</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>